<commit_message>
Fix: slow_mvmnt msg did excess circshift in run_q.m, so events weren't aligned to timestamps
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/trial_lists/practice_wo_prime_trials.xlsx
+++ b/experiment/RUN_ME/stimuli/trial_lists/practice_wo_prime_trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\trial_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5103AFAC-752C-449A-96C8-E1A2FE031F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446454E6-7299-4758-9A61-FB7DC7D424D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BADE156A-26C9-4C97-926F-835B0ED8E3B4}"/>
   </bookViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD1C534-B53B-4F86-80A4-21D2A94799B7}">
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -959,22 +959,22 @@
         <v>42</v>
       </c>
       <c r="Q2">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S2">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T2">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U2">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V2">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -1027,22 +1027,22 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S3">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T3">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U3">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V3">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO3">
         <v>0</v>
@@ -1095,22 +1095,22 @@
         <v>59</v>
       </c>
       <c r="Q4">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S4">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T4">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U4">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V4">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO4">
         <v>0</v>
@@ -1163,22 +1163,22 @@
         <v>47</v>
       </c>
       <c r="Q5">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S5">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T5">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U5">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V5">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO5">
         <v>0</v>
@@ -1231,22 +1231,22 @@
         <v>39</v>
       </c>
       <c r="Q6">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S6">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T6">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U6">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V6">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO6">
         <v>0</v>
@@ -1299,22 +1299,22 @@
         <v>24</v>
       </c>
       <c r="Q7">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S7">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T7">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U7">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V7">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO7">
         <v>0</v>
@@ -1367,22 +1367,22 @@
         <v>32</v>
       </c>
       <c r="Q8">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R8">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S8">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T8">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U8">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V8">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO8">
         <v>0</v>
@@ -1435,22 +1435,22 @@
         <v>8</v>
       </c>
       <c r="Q9">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S9">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T9">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U9">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V9">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO9">
         <v>0</v>
@@ -1503,22 +1503,22 @@
         <v>58</v>
       </c>
       <c r="Q10">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S10">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T10">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U10">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V10">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO10">
         <v>0</v>
@@ -1571,22 +1571,22 @@
         <v>15</v>
       </c>
       <c r="Q11">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S11">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T11">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U11">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V11">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO11">
         <v>0</v>
@@ -1639,22 +1639,22 @@
         <v>42</v>
       </c>
       <c r="Q12">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S12">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T12">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U12">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V12">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO12">
         <v>0</v>
@@ -1707,22 +1707,22 @@
         <v>4</v>
       </c>
       <c r="Q13">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S13">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T13">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U13">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V13">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO13">
         <v>0</v>
@@ -1775,22 +1775,22 @@
         <v>46</v>
       </c>
       <c r="Q14">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S14">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T14">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U14">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V14">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO14">
         <v>0</v>
@@ -1843,22 +1843,22 @@
         <v>49</v>
       </c>
       <c r="Q15">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S15">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T15">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U15">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V15">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO15">
         <v>0</v>
@@ -1911,22 +1911,22 @@
         <v>13</v>
       </c>
       <c r="Q16">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R16">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S16">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T16">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U16">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V16">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO16">
         <v>0</v>
@@ -1979,22 +1979,22 @@
         <v>32</v>
       </c>
       <c r="Q17">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S17">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T17">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U17">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V17">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO17">
         <v>0</v>
@@ -2047,22 +2047,22 @@
         <v>19</v>
       </c>
       <c r="Q18">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R18">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S18">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T18">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U18">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V18">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO18">
         <v>0</v>
@@ -2115,22 +2115,22 @@
         <v>37</v>
       </c>
       <c r="Q19">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S19">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T19">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U19">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V19">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO19">
         <v>0</v>
@@ -2183,22 +2183,22 @@
         <v>30</v>
       </c>
       <c r="Q20">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R20">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S20">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T20">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U20">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V20">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO20">
         <v>0</v>
@@ -2251,22 +2251,22 @@
         <v>16</v>
       </c>
       <c r="Q21">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S21">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T21">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U21">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V21">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO21">
         <v>0</v>
@@ -2319,22 +2319,22 @@
         <v>29</v>
       </c>
       <c r="Q22">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S22">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T22">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U22">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V22">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO22">
         <v>0</v>
@@ -2387,22 +2387,22 @@
         <v>12</v>
       </c>
       <c r="Q23">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R23">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S23">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T23">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U23">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V23">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO23">
         <v>0</v>
@@ -2455,22 +2455,22 @@
         <v>51</v>
       </c>
       <c r="Q24">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R24">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S24">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T24">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U24">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V24">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO24">
         <v>0</v>
@@ -2523,22 +2523,22 @@
         <v>59</v>
       </c>
       <c r="Q25">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R25">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S25">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T25">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U25">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V25">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO25">
         <v>0</v>
@@ -2591,22 +2591,22 @@
         <v>29</v>
       </c>
       <c r="Q26">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R26">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S26">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T26">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U26">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V26">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO26">
         <v>0</v>
@@ -2659,22 +2659,22 @@
         <v>7</v>
       </c>
       <c r="Q27">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R27">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S27">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T27">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U27">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V27">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO27">
         <v>0</v>
@@ -2727,22 +2727,22 @@
         <v>20</v>
       </c>
       <c r="Q28">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R28">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S28">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T28">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U28">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V28">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO28">
         <v>0</v>
@@ -2795,22 +2795,22 @@
         <v>51</v>
       </c>
       <c r="Q29">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R29">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S29">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T29">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U29">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V29">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO29">
         <v>0</v>
@@ -2863,22 +2863,22 @@
         <v>31</v>
       </c>
       <c r="Q30">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R30">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S30">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T30">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U30">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V30">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO30">
         <v>0</v>
@@ -2931,22 +2931,22 @@
         <v>44</v>
       </c>
       <c r="Q31">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R31">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S31">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T31">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U31">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V31">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO31">
         <v>0</v>
@@ -2999,22 +2999,22 @@
         <v>38</v>
       </c>
       <c r="Q32">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R32">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S32">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T32">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U32">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V32">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO32">
         <v>0</v>
@@ -3067,22 +3067,22 @@
         <v>26</v>
       </c>
       <c r="Q33">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R33">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S33">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T33">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U33">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V33">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO33">
         <v>0</v>
@@ -3135,22 +3135,22 @@
         <v>29</v>
       </c>
       <c r="Q34">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R34">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S34">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T34">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U34">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V34">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO34">
         <v>0</v>
@@ -3203,22 +3203,22 @@
         <v>45</v>
       </c>
       <c r="Q35">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R35">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S35">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T35">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U35">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V35">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO35">
         <v>0</v>
@@ -3271,22 +3271,22 @@
         <v>2</v>
       </c>
       <c r="Q36">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R36">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S36">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T36">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U36">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V36">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO36">
         <v>0</v>
@@ -3339,22 +3339,22 @@
         <v>49</v>
       </c>
       <c r="Q37">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R37">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S37">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T37">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U37">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V37">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO37">
         <v>0</v>
@@ -3407,22 +3407,22 @@
         <v>34</v>
       </c>
       <c r="Q38">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R38">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S38">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T38">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U38">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V38">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO38">
         <v>0</v>
@@ -3475,22 +3475,22 @@
         <v>59</v>
       </c>
       <c r="Q39">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R39">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S39">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T39">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U39">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V39">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO39">
         <v>0</v>
@@ -3543,22 +3543,22 @@
         <v>13</v>
       </c>
       <c r="Q40">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R40">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S40">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T40">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U40">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V40">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO40">
         <v>0</v>
@@ -3611,22 +3611,22 @@
         <v>56</v>
       </c>
       <c r="Q41">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R41">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S41">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T41">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U41">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V41">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO41">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "Fix: slow_mvmnt msg did excess circshift in run_q.m, so events weren't aligned to timestamps"
This reverts commit 6ad27918439f05cb3fd45c7f5515f3cee57f113b.
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/trial_lists/practice_wo_prime_trials.xlsx
+++ b/experiment/RUN_ME/stimuli/trial_lists/practice_wo_prime_trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\trial_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446454E6-7299-4758-9A61-FB7DC7D424D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5103AFAC-752C-449A-96C8-E1A2FE031F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BADE156A-26C9-4C97-926F-835B0ED8E3B4}"/>
   </bookViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD1C534-B53B-4F86-80A4-21D2A94799B7}">
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -959,22 +959,22 @@
         <v>42</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R2">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S2">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T2">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U2">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -1027,22 +1027,22 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R3">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S3">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T3">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U3">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO3">
         <v>0</v>
@@ -1095,22 +1095,22 @@
         <v>59</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R4">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S4">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T4">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U4">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V4">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO4">
         <v>0</v>
@@ -1163,22 +1163,22 @@
         <v>47</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R5">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S5">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T5">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U5">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V5">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO5">
         <v>0</v>
@@ -1231,22 +1231,22 @@
         <v>39</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R6">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S6">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T6">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U6">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V6">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO6">
         <v>0</v>
@@ -1299,22 +1299,22 @@
         <v>24</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R7">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S7">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T7">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U7">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V7">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO7">
         <v>0</v>
@@ -1367,22 +1367,22 @@
         <v>32</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R8">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S8">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T8">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U8">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V8">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO8">
         <v>0</v>
@@ -1435,22 +1435,22 @@
         <v>8</v>
       </c>
       <c r="Q9">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R9">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S9">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T9">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U9">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V9">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO9">
         <v>0</v>
@@ -1503,22 +1503,22 @@
         <v>58</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R10">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S10">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T10">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U10">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V10">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO10">
         <v>0</v>
@@ -1571,22 +1571,22 @@
         <v>15</v>
       </c>
       <c r="Q11">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R11">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S11">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T11">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U11">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V11">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO11">
         <v>0</v>
@@ -1639,22 +1639,22 @@
         <v>42</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R12">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S12">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T12">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U12">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V12">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO12">
         <v>0</v>
@@ -1707,22 +1707,22 @@
         <v>4</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R13">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S13">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T13">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U13">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V13">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO13">
         <v>0</v>
@@ -1775,22 +1775,22 @@
         <v>46</v>
       </c>
       <c r="Q14">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R14">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S14">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T14">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U14">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V14">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO14">
         <v>0</v>
@@ -1843,22 +1843,22 @@
         <v>49</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R15">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S15">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T15">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U15">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V15">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO15">
         <v>0</v>
@@ -1911,22 +1911,22 @@
         <v>13</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R16">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S16">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T16">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U16">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V16">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO16">
         <v>0</v>
@@ -1979,22 +1979,22 @@
         <v>32</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R17">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S17">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T17">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U17">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V17">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO17">
         <v>0</v>
@@ -2047,22 +2047,22 @@
         <v>19</v>
       </c>
       <c r="Q18">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R18">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S18">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T18">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U18">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V18">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO18">
         <v>0</v>
@@ -2115,22 +2115,22 @@
         <v>37</v>
       </c>
       <c r="Q19">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R19">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S19">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T19">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U19">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V19">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO19">
         <v>0</v>
@@ -2183,22 +2183,22 @@
         <v>30</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R20">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S20">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T20">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U20">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V20">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO20">
         <v>0</v>
@@ -2251,22 +2251,22 @@
         <v>16</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R21">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S21">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T21">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U21">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V21">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO21">
         <v>0</v>
@@ -2319,22 +2319,22 @@
         <v>29</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R22">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S22">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T22">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U22">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V22">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO22">
         <v>0</v>
@@ -2387,22 +2387,22 @@
         <v>12</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R23">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S23">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T23">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U23">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V23">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO23">
         <v>0</v>
@@ -2455,22 +2455,22 @@
         <v>51</v>
       </c>
       <c r="Q24">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R24">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S24">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T24">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U24">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V24">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO24">
         <v>0</v>
@@ -2523,22 +2523,22 @@
         <v>59</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R25">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S25">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T25">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U25">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V25">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO25">
         <v>0</v>
@@ -2591,22 +2591,22 @@
         <v>29</v>
       </c>
       <c r="Q26">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R26">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S26">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T26">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U26">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V26">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO26">
         <v>0</v>
@@ -2659,22 +2659,22 @@
         <v>7</v>
       </c>
       <c r="Q27">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R27">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S27">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T27">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U27">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V27">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO27">
         <v>0</v>
@@ -2727,22 +2727,22 @@
         <v>20</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R28">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S28">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T28">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U28">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V28">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO28">
         <v>0</v>
@@ -2795,22 +2795,22 @@
         <v>51</v>
       </c>
       <c r="Q29">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R29">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S29">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T29">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U29">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V29">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO29">
         <v>0</v>
@@ -2863,22 +2863,22 @@
         <v>31</v>
       </c>
       <c r="Q30">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R30">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S30">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T30">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U30">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V30">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO30">
         <v>0</v>
@@ -2931,22 +2931,22 @@
         <v>44</v>
       </c>
       <c r="Q31">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R31">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S31">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T31">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U31">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V31">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO31">
         <v>0</v>
@@ -2999,22 +2999,22 @@
         <v>38</v>
       </c>
       <c r="Q32">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R32">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S32">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T32">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U32">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V32">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO32">
         <v>0</v>
@@ -3067,22 +3067,22 @@
         <v>26</v>
       </c>
       <c r="Q33">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R33">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S33">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T33">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U33">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V33">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO33">
         <v>0</v>
@@ -3135,22 +3135,22 @@
         <v>29</v>
       </c>
       <c r="Q34">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R34">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S34">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T34">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U34">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V34">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO34">
         <v>0</v>
@@ -3203,22 +3203,22 @@
         <v>45</v>
       </c>
       <c r="Q35">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R35">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S35">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T35">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U35">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V35">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO35">
         <v>0</v>
@@ -3271,22 +3271,22 @@
         <v>2</v>
       </c>
       <c r="Q36">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R36">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S36">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T36">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U36">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V36">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO36">
         <v>0</v>
@@ -3339,22 +3339,22 @@
         <v>49</v>
       </c>
       <c r="Q37">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R37">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S37">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T37">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U37">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V37">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO37">
         <v>0</v>
@@ -3407,22 +3407,22 @@
         <v>34</v>
       </c>
       <c r="Q38">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R38">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S38">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T38">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U38">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V38">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO38">
         <v>0</v>
@@ -3475,22 +3475,22 @@
         <v>59</v>
       </c>
       <c r="Q39">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R39">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S39">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T39">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U39">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V39">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO39">
         <v>0</v>
@@ -3543,22 +3543,22 @@
         <v>13</v>
       </c>
       <c r="Q40">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R40">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S40">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T40">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U40">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V40">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO40">
         <v>0</v>
@@ -3611,22 +3611,22 @@
         <v>56</v>
       </c>
       <c r="Q41">
-        <v>1</v>
+        <v>0.98750000000000004</v>
       </c>
       <c r="R41">
-        <v>0.27</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="S41">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="T41">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="U41">
-        <v>0.03</v>
+        <v>1.7499999999999998E-2</v>
       </c>
       <c r="V41">
-        <v>0.5</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="AO41">
         <v>0</v>

</xml_diff>

<commit_message>
Fix dates in subject_log | fix duration in trials list
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/trial_lists/practice_wo_prime_trials.xlsx
+++ b/experiment/RUN_ME/stimuli/trial_lists/practice_wo_prime_trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\trial_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5103AFAC-752C-449A-96C8-E1A2FE031F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446454E6-7299-4758-9A61-FB7DC7D424D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BADE156A-26C9-4C97-926F-835B0ED8E3B4}"/>
   </bookViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD1C534-B53B-4F86-80A4-21D2A94799B7}">
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -959,22 +959,22 @@
         <v>42</v>
       </c>
       <c r="Q2">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R2">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S2">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T2">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U2">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V2">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO2">
         <v>0</v>
@@ -1027,22 +1027,22 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S3">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T3">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U3">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V3">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO3">
         <v>0</v>
@@ -1095,22 +1095,22 @@
         <v>59</v>
       </c>
       <c r="Q4">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R4">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S4">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T4">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U4">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V4">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO4">
         <v>0</v>
@@ -1163,22 +1163,22 @@
         <v>47</v>
       </c>
       <c r="Q5">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R5">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S5">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T5">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U5">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V5">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO5">
         <v>0</v>
@@ -1231,22 +1231,22 @@
         <v>39</v>
       </c>
       <c r="Q6">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S6">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T6">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U6">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V6">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO6">
         <v>0</v>
@@ -1299,22 +1299,22 @@
         <v>24</v>
       </c>
       <c r="Q7">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R7">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S7">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T7">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U7">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V7">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO7">
         <v>0</v>
@@ -1367,22 +1367,22 @@
         <v>32</v>
       </c>
       <c r="Q8">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R8">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S8">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T8">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U8">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V8">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO8">
         <v>0</v>
@@ -1435,22 +1435,22 @@
         <v>8</v>
       </c>
       <c r="Q9">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R9">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S9">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T9">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U9">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V9">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO9">
         <v>0</v>
@@ -1503,22 +1503,22 @@
         <v>58</v>
       </c>
       <c r="Q10">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S10">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T10">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U10">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V10">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO10">
         <v>0</v>
@@ -1571,22 +1571,22 @@
         <v>15</v>
       </c>
       <c r="Q11">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S11">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T11">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U11">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V11">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO11">
         <v>0</v>
@@ -1639,22 +1639,22 @@
         <v>42</v>
       </c>
       <c r="Q12">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S12">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T12">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U12">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V12">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO12">
         <v>0</v>
@@ -1707,22 +1707,22 @@
         <v>4</v>
       </c>
       <c r="Q13">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R13">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S13">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T13">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U13">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V13">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO13">
         <v>0</v>
@@ -1775,22 +1775,22 @@
         <v>46</v>
       </c>
       <c r="Q14">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R14">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S14">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T14">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U14">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V14">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO14">
         <v>0</v>
@@ -1843,22 +1843,22 @@
         <v>49</v>
       </c>
       <c r="Q15">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S15">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T15">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U15">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V15">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO15">
         <v>0</v>
@@ -1911,22 +1911,22 @@
         <v>13</v>
       </c>
       <c r="Q16">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R16">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S16">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T16">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U16">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V16">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO16">
         <v>0</v>
@@ -1979,22 +1979,22 @@
         <v>32</v>
       </c>
       <c r="Q17">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S17">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T17">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U17">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V17">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO17">
         <v>0</v>
@@ -2047,22 +2047,22 @@
         <v>19</v>
       </c>
       <c r="Q18">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R18">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S18">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T18">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U18">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V18">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO18">
         <v>0</v>
@@ -2115,22 +2115,22 @@
         <v>37</v>
       </c>
       <c r="Q19">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R19">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S19">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T19">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U19">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V19">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO19">
         <v>0</v>
@@ -2183,22 +2183,22 @@
         <v>30</v>
       </c>
       <c r="Q20">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R20">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S20">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T20">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U20">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V20">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO20">
         <v>0</v>
@@ -2251,22 +2251,22 @@
         <v>16</v>
       </c>
       <c r="Q21">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R21">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S21">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T21">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U21">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V21">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO21">
         <v>0</v>
@@ -2319,22 +2319,22 @@
         <v>29</v>
       </c>
       <c r="Q22">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R22">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S22">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T22">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U22">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V22">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO22">
         <v>0</v>
@@ -2387,22 +2387,22 @@
         <v>12</v>
       </c>
       <c r="Q23">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R23">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S23">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T23">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U23">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V23">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO23">
         <v>0</v>
@@ -2455,22 +2455,22 @@
         <v>51</v>
       </c>
       <c r="Q24">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R24">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S24">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T24">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U24">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V24">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO24">
         <v>0</v>
@@ -2523,22 +2523,22 @@
         <v>59</v>
       </c>
       <c r="Q25">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R25">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S25">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T25">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U25">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V25">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO25">
         <v>0</v>
@@ -2591,22 +2591,22 @@
         <v>29</v>
       </c>
       <c r="Q26">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R26">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S26">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T26">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U26">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V26">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO26">
         <v>0</v>
@@ -2659,22 +2659,22 @@
         <v>7</v>
       </c>
       <c r="Q27">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R27">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S27">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T27">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U27">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V27">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO27">
         <v>0</v>
@@ -2727,22 +2727,22 @@
         <v>20</v>
       </c>
       <c r="Q28">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R28">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S28">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T28">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U28">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V28">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO28">
         <v>0</v>
@@ -2795,22 +2795,22 @@
         <v>51</v>
       </c>
       <c r="Q29">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R29">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S29">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T29">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U29">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V29">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO29">
         <v>0</v>
@@ -2863,22 +2863,22 @@
         <v>31</v>
       </c>
       <c r="Q30">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R30">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S30">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T30">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U30">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V30">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO30">
         <v>0</v>
@@ -2931,22 +2931,22 @@
         <v>44</v>
       </c>
       <c r="Q31">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R31">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S31">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T31">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U31">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V31">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO31">
         <v>0</v>
@@ -2999,22 +2999,22 @@
         <v>38</v>
       </c>
       <c r="Q32">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R32">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S32">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T32">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U32">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V32">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO32">
         <v>0</v>
@@ -3067,22 +3067,22 @@
         <v>26</v>
       </c>
       <c r="Q33">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R33">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S33">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T33">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U33">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V33">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO33">
         <v>0</v>
@@ -3135,22 +3135,22 @@
         <v>29</v>
       </c>
       <c r="Q34">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R34">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S34">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T34">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U34">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V34">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO34">
         <v>0</v>
@@ -3203,22 +3203,22 @@
         <v>45</v>
       </c>
       <c r="Q35">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R35">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S35">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T35">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U35">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V35">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO35">
         <v>0</v>
@@ -3271,22 +3271,22 @@
         <v>2</v>
       </c>
       <c r="Q36">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R36">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S36">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T36">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U36">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V36">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO36">
         <v>0</v>
@@ -3339,22 +3339,22 @@
         <v>49</v>
       </c>
       <c r="Q37">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R37">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S37">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T37">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U37">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V37">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO37">
         <v>0</v>
@@ -3407,22 +3407,22 @@
         <v>34</v>
       </c>
       <c r="Q38">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R38">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S38">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T38">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U38">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V38">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO38">
         <v>0</v>
@@ -3475,22 +3475,22 @@
         <v>59</v>
       </c>
       <c r="Q39">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R39">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S39">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T39">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U39">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V39">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO39">
         <v>0</v>
@@ -3543,22 +3543,22 @@
         <v>13</v>
       </c>
       <c r="Q40">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R40">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S40">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T40">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U40">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V40">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO40">
         <v>0</v>
@@ -3611,22 +3611,22 @@
         <v>56</v>
       </c>
       <c r="Q41">
-        <v>0.98750000000000004</v>
+        <v>1</v>
       </c>
       <c r="R41">
-        <v>0.25750000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="S41">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="T41">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="U41">
-        <v>1.7499999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="V41">
-        <v>0.48749999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="AO41">
         <v>0</v>

</xml_diff>